<commit_message>
new dic, counted till 2010
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -503,37 +503,37 @@
         <v>1865</v>
       </c>
       <c r="C2" t="n">
-        <v>9</v>
+        <v>172</v>
       </c>
       <c r="D2" t="n">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="E2" t="n">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="F2" t="n">
         <v>6</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J2" t="n">
         <v>310</v>
       </c>
       <c r="K2" t="n">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="L2" t="n">
         <v>119</v>
       </c>
       <c r="M2" t="n">
-        <v>14</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3">
@@ -541,40 +541,40 @@
         <v>2009</v>
       </c>
       <c r="B3" t="n">
-        <v>1793</v>
+        <v>1794</v>
       </c>
       <c r="C3" t="n">
-        <v>98</v>
+        <v>372</v>
       </c>
       <c r="D3" t="n">
-        <v>923</v>
+        <v>930</v>
       </c>
       <c r="E3" t="n">
-        <v>100</v>
+        <v>257</v>
       </c>
       <c r="F3" t="n">
         <v>6</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J3" t="n">
         <v>362</v>
       </c>
       <c r="K3" t="n">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="L3" t="n">
         <v>161</v>
       </c>
       <c r="M3" t="n">
-        <v>9</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4">
@@ -585,37 +585,37 @@
         <v>2715</v>
       </c>
       <c r="C4" t="n">
-        <v>46</v>
+        <v>412</v>
       </c>
       <c r="D4" t="n">
-        <v>1057</v>
+        <v>1067</v>
       </c>
       <c r="E4" t="n">
-        <v>253</v>
+        <v>467</v>
       </c>
       <c r="F4" t="n">
         <v>11</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J4" t="n">
         <v>666</v>
       </c>
       <c r="K4" t="n">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="L4" t="n">
         <v>152</v>
       </c>
       <c r="M4" t="n">
-        <v>13</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5">

</xml_diff>